<commit_message>
Adding the EC-Earth ES-DOC documentantion content which has been collected across the EC-Earth consortium at the end of the third EC-Earth ES-DOC documentantion session via shared google-doc documents.
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_ec-earth-consortium_citations.xlsx
+++ b/cmip6/citations/cmip6_ec-earth-consortium_citations.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjD58a97KRxswnIq9w26fkDu6Cv3w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhgzcRS9w7J5s7dRmlhtOZpWaYd4A=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -80,12 +80,22 @@
     <t>Doescher-et-al-2020</t>
   </si>
   <si>
-    <t>"@article{
-  title = {The Community Earth System Model EC-Earth for collaborative climate research},
-  journal = {Geoscientific Model Development Discussions},
-  author = {Döscher, v. Hardenberg, Wyser, v. Noije, Le Sager, Fladrich, Koenigk, O’Donnell, Miller, Gröger, Menegoz … Carver, Bousetta, Almut Arneth, Louis-Philippe Caron, Raffa Bernardello , Valentina, Etienne, Pablo Ortega, Uotila, Eleftheria, Mario …, Paul Nolan, … Gijs van den Oord, Thomas Reerink, Lars Nieradzik and Tommi Bergman , Peter Anthoni,  David Wårlind, Ben Smith ‎… many others.},
-  year = {2020},
-}"</t>
+    <t>10.5194/gmd-2020-446</t>
+  </si>
+  <si>
+    <t>@Article{gmd-2020-446,
+AUTHOR = {Ralf Döscher, Mario Acosta, Andrea Alessandri, Peter Anthoni, Almut Arneth, Thomas Arsouze, Tommi Bergmann, Raffaele Bernadello, Souhail Bousetta, Louis-Philippe Caron, Glenn Carver, Miguel Castrillo, Franco Catalano, Ivana Cvijanovic, Paolo Davini, Evelien Dekker, Francisco J. Doblas-Reyes, David Docquier, Pablo Echevarria, Uwe Fladrich, Ramon Fuentes-Franco, Matthias Gröger, Jost v. Hardenberg, Jenny Hieronymus, M. Pasha Karami, Jukka-Pekka Keskinen, Torben Koenigk, Risto Makkonen, Francois Massonnet, Martin Ménégoz, Paul A. Miller, Eduardo Moreno-Chamarro, Lars Nieradzik, Twan van Noije, Paul Nolan, Declan O’Donnell, Pirrka Ollinaho, Gijs van den Oord, Oriol Tintó Prims, Arthur Ramos, Thomas Reerink, Clement Rousset, Yohan Ruprich-Robert, Philippe Le Sager, Torben Schmith, Roland Schrödner, Federico Serva, Valentina Sicardi, Marianne Sloth Madsen, Benjamin Smith, Tian Tian, Etienne Tourigny, Petteri Uotila, Martin Vancoppenolle, Shiyu Wang, David Wårlind, Ulrika Willén, Klaus Wyser, Shuting Yang, and Xavier Yepes-Arbós},
+TITLE = {The EC-Earth3 Earth System Model for the Climate Model Intercomparison Project 6},
+JOURNAL = {Geoscientific Model Development Discussions},
+VOLUME = {2021},
+YEAR = {2021},
+PAGES = {},
+URL = {https://gmd.copernicus.org/preprints/gmd-2020-446/},
+DOI = {10.5194/gmd-2020-446}
+}</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5194/gmd-2020-446</t>
   </si>
   <si>
     <t>Hazeleger-et-al-2012</t>
@@ -152,12 +162,23 @@
     <t>van-Noije-et-al-2020</t>
   </si>
   <si>
-    <t>@Article{,
-AUTHOR = {van Noije, T. P. C. and Le Sager, P. and others},
-TITLE = {EC-Earth3-AerChem, a global climate model with interactive aerosols and atmospheric chemistry participating in CMIP6},
+    <t>10.5194/gmd-2020-413</t>
+  </si>
+  <si>
+    <t>@Article{gmd-2020-413,
+AUTHOR = {van Noije, T. and Bergman, T. and Le Sager, P. and O'Donnell, D. and Makkonen, R. and Gon\c{c}alves-Ageitos, M. and D\"oscher, R. and Fladrich, U. and von Hardenberg, J. and Keskinen, J.-P. and Korhonen, H. and Laakso, A. and Myriokefalitakis, S. and Ollinaho, P. and P\'erez Garc\'{\i}a-Pando, C. and Reerink, T. and Schr\"odner, R. and Wyser, K. and Yang, S.},
+TITLE = {EC-Earth3-AerChem, a global climate model with interactive aerosols
+and atmospheric chemistry participating in CMIP6},
 JOURNAL = {Geoscientific Model Development Discussions},
-YEAR = {2020}
+VOLUME = {2020},
+YEAR = {2020},
+PAGES = {1--46},
+URL = {https://gmd.copernicus.org/preprints/gmd-2020-413/},
+DOI = {10.5194/gmd-2020-413}
 }</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5194/gmd-2020-413</t>
   </si>
   <si>
     <t>Wyser-et-al-2019</t>
@@ -419,7 +440,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -487,12 +508,26 @@
       <name val="Roboto"/>
     </font>
     <font>
+      <i/>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <u/>
       <color rgb="FF0000FF"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF464646"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF464646"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -518,13 +553,13 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF2A2D35"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="6">
@@ -658,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -725,62 +760,56 @@
     <xf borderId="10" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="5" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="5" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13951,11 +13980,15 @@
       <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="C3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="E3" s="16"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
@@ -13980,16 +14013,16 @@
     </row>
     <row r="4" ht="129.0" customHeight="1">
       <c r="A4" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>18</v>
+      <c r="B4" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>20</v>
+      <c r="D4" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
@@ -14015,16 +14048,16 @@
     </row>
     <row r="5" ht="129.0" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>22</v>
+      <c r="B5" s="25" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>24</v>
+      <c r="D5" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
@@ -14050,13 +14083,17 @@
     </row>
     <row r="6" ht="129.0" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="16" t="s">
-        <v>26</v>
+      <c r="B6" s="27" t="s">
+        <v>28</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="C6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" s="16"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -14081,16 +14118,16 @@
     </row>
     <row r="7" ht="129.0" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>28</v>
+      <c r="B7" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>30</v>
+      <c r="D7" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="17"/>
@@ -14115,11 +14152,11 @@
       <c r="Y7" s="17"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="25" t="s">
-        <v>31</v>
+      <c r="A8" s="29" t="s">
+        <v>35</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>32</v>
+      <c r="B8" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -14146,11 +14183,11 @@
       <c r="Y8" s="13"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="25" t="s">
-        <v>33</v>
+      <c r="A9" s="29" t="s">
+        <v>37</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>34</v>
+      <c r="B9" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -14177,11 +14214,11 @@
       <c r="Y9" s="13"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="28" t="s">
-        <v>35</v>
+      <c r="A10" s="32" t="s">
+        <v>39</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>36</v>
+      <c r="B10" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -14208,11 +14245,11 @@
       <c r="Y10" s="13"/>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="28" t="s">
-        <v>37</v>
+      <c r="A11" s="32" t="s">
+        <v>41</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>38</v>
+      <c r="B11" s="31" t="s">
+        <v>42</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -14240,16 +14277,16 @@
     </row>
     <row r="12" ht="79.5" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>42</v>
+      <c r="D12" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="13"/>
@@ -14275,16 +14312,16 @@
     </row>
     <row r="13" ht="112.5" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>46</v>
+      <c r="D13" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="13"/>
@@ -14310,16 +14347,16 @@
     </row>
     <row r="14" ht="126.0" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>48</v>
+      <c r="B14" s="34" t="s">
+        <v>52</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
-      <c r="D14" s="29" t="s">
-        <v>50</v>
+      <c r="D14" s="33" t="s">
+        <v>54</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="13"/>
@@ -14344,17 +14381,17 @@
       <c r="Y14" s="13"/>
     </row>
     <row r="15" ht="69.0" customHeight="1">
-      <c r="A15" s="31" t="s">
-        <v>51</v>
+      <c r="A15" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>54</v>
+      <c r="D15" s="33" t="s">
+        <v>58</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="13"/>
@@ -14380,11 +14417,11 @@
     </row>
     <row r="16" ht="75.0" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -14410,11 +14447,11 @@
       <c r="Y16" s="13"/>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="32" t="s">
-        <v>57</v>
+      <c r="A17" s="18" t="s">
+        <v>61</v>
       </c>
-      <c r="B17" s="33" t="s">
-        <v>58</v>
+      <c r="B17" s="36" t="s">
+        <v>62</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -14441,11 +14478,11 @@
       <c r="Y17" s="13"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="32" t="s">
-        <v>59</v>
+      <c r="A18" s="18" t="s">
+        <v>63</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>60</v>
+      <c r="B18" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -14472,11 +14509,11 @@
       <c r="Y18" s="13"/>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="32" t="s">
-        <v>61</v>
+      <c r="A19" s="18" t="s">
+        <v>65</v>
       </c>
-      <c r="B19" s="34" t="s">
-        <v>62</v>
+      <c r="B19" s="37" t="s">
+        <v>66</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -14503,11 +14540,11 @@
       <c r="Y19" s="13"/>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="32" t="s">
-        <v>63</v>
+      <c r="A20" s="18" t="s">
+        <v>67</v>
       </c>
-      <c r="B20" s="34" t="s">
-        <v>64</v>
+      <c r="B20" s="37" t="s">
+        <v>68</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -14534,11 +14571,11 @@
       <c r="Y20" s="13"/>
     </row>
     <row r="21" ht="19.5" customHeight="1">
-      <c r="A21" s="32" t="s">
-        <v>65</v>
+      <c r="A21" s="18" t="s">
+        <v>69</v>
       </c>
-      <c r="B21" s="34" t="s">
-        <v>66</v>
+      <c r="B21" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -14565,12 +14602,12 @@
       <c r="Y21" s="13"/>
     </row>
     <row r="22" ht="55.5" customHeight="1">
-      <c r="A22" s="35" t="s">
-        <v>67</v>
+      <c r="A22" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="B22" s="21"/>
-      <c r="C22" s="36" t="s">
-        <v>68</v>
+      <c r="C22" s="38" t="s">
+        <v>72</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -14596,17 +14633,17 @@
       <c r="Y22" s="13"/>
     </row>
     <row r="23" ht="129.0" customHeight="1">
-      <c r="A23" s="37" t="s">
-        <v>69</v>
+      <c r="A23" s="15" t="s">
+        <v>73</v>
       </c>
-      <c r="B23" s="38" t="s">
-        <v>70</v>
+      <c r="B23" s="25" t="s">
+        <v>74</v>
       </c>
-      <c r="C23" s="39" t="s">
-        <v>71</v>
+      <c r="C23" s="16" t="s">
+        <v>75</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>72</v>
+      <c r="D23" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="17"/>
@@ -14631,17 +14668,17 @@
       <c r="Y23" s="17"/>
     </row>
     <row r="24" ht="129.0" customHeight="1">
-      <c r="A24" s="37" t="s">
-        <v>47</v>
+      <c r="A24" s="15" t="s">
+        <v>51</v>
       </c>
-      <c r="B24" s="38" t="s">
-        <v>48</v>
+      <c r="B24" s="25" t="s">
+        <v>52</v>
       </c>
-      <c r="C24" s="39" t="s">
-        <v>73</v>
+      <c r="C24" s="16" t="s">
+        <v>77</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>74</v>
+      <c r="D24" s="26" t="s">
+        <v>78</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="17"/>
@@ -20739,15 +20776,18 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D4"/>
-    <hyperlink r:id="rId2" ref="D5"/>
-    <hyperlink r:id="rId3" ref="D7"/>
-    <hyperlink r:id="rId4" ref="D12"/>
-    <hyperlink r:id="rId5" ref="D13"/>
-    <hyperlink r:id="rId6" ref="D14"/>
-    <hyperlink r:id="rId7" ref="D15"/>
-    <hyperlink r:id="rId8" ref="D23"/>
-    <hyperlink r:id="rId9" ref="D24"/>
+    <hyperlink r:id="rId1" ref="D3"/>
+    <hyperlink r:id="rId2" ref="D4"/>
+    <hyperlink r:id="rId3" ref="D5"/>
+    <hyperlink r:id="rId4" ref="B6"/>
+    <hyperlink r:id="rId5" ref="D6"/>
+    <hyperlink r:id="rId6" ref="D7"/>
+    <hyperlink r:id="rId7" ref="D12"/>
+    <hyperlink r:id="rId8" ref="D13"/>
+    <hyperlink r:id="rId9" ref="D14"/>
+    <hyperlink r:id="rId10" ref="D15"/>
+    <hyperlink r:id="rId11" ref="D23"/>
+    <hyperlink r:id="rId12" ref="D24"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.5" right="0.5" top="0.75"/>
@@ -20755,6 +20795,6 @@
   <headerFooter>
     <oddFooter>&amp;C000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>